<commit_message>
new excel for dictionary engine - mountains.xlsx rename for dictionary buttons - buttons_geography.xml
</commit_message>
<xml_diff>
--- a/SchVictorina.WebAPI/Config/mountains.xlsx
+++ b/SchVictorina.WebAPI/Config/mountains.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\schvictorina\schvictorina\SchVictorina.WebAPI\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ECFCDA04-8E99-4BF4-88C6-D80A8A639D95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{717FBB7B-EEAC-45C9-8722-52CFB2D3DE98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{58996942-A194-4CF7-8E0B-222C89F5D031}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{58996942-A194-4CF7-8E0B-222C89F5D031}"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Данные" sheetId="1" r:id="rId1"/>
+    <sheet name="Вопросы" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Лист1!$A$1:$E$18</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Данные!$A$1:$E$16</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="44">
   <si>
     <t>Название</t>
   </si>
@@ -46,9 +47,6 @@
     <t>Высота</t>
   </si>
   <si>
-    <t>Местоположение</t>
-  </si>
-  <si>
     <t>Первое восхождение</t>
   </si>
   <si>
@@ -70,12 +68,6 @@
     <t>Европа</t>
   </si>
   <si>
-    <t>Драконские горы</t>
-  </si>
-  <si>
-    <t>Каспийские горы</t>
-  </si>
-  <si>
     <t>Горы Атлас</t>
   </si>
   <si>
@@ -88,9 +80,6 @@
     <t>Гималаи</t>
   </si>
   <si>
-    <t>Японские Альпы</t>
-  </si>
-  <si>
     <t>Тянь-Шань</t>
   </si>
   <si>
@@ -115,17 +104,80 @@
     <t>Пиренеи</t>
   </si>
   <si>
-    <t>Балканские горы</t>
-  </si>
-  <si>
     <t>Татры</t>
+  </si>
+  <si>
+    <t>Россия</t>
+  </si>
+  <si>
+    <t>Италия</t>
+  </si>
+  <si>
+    <t>Китай</t>
+  </si>
+  <si>
+    <t>Марокко</t>
+  </si>
+  <si>
+    <t>Драконовы горы</t>
+  </si>
+  <si>
+    <t>ЮАР</t>
+  </si>
+  <si>
+    <t>Польша</t>
+  </si>
+  <si>
+    <t>Капские горы</t>
+  </si>
+  <si>
+    <t>question</t>
+  </si>
+  <si>
+    <t>filter</t>
+  </si>
+  <si>
+    <t>equal</t>
+  </si>
+  <si>
+    <t>orderBy</t>
+  </si>
+  <si>
+    <t>orderByDesc</t>
+  </si>
+  <si>
+    <t>answer</t>
+  </si>
+  <si>
+    <t>Какая самая высокая гора в {Континент}</t>
+  </si>
+  <si>
+    <t>Какую гору покорили первой в {Континент}</t>
+  </si>
+  <si>
+    <t>Какую гору покорили первой</t>
+  </si>
+  <si>
+    <t>Аргентина</t>
+  </si>
+  <si>
+    <t>Испания</t>
+  </si>
+  <si>
+    <t>Какая самая высокая гора в {Страна}</t>
+  </si>
+  <si>
+    <t>Страна</t>
+  </si>
+  <si>
+    <t>Новая зеландия</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,8 +194,24 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF202122"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFBDC1C6"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -153,6 +221,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -169,12 +243,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -489,184 +568,399 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56986E0B-A4A6-4723-A20F-D2A7B21D0681}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.109375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="6">
+        <v>4509</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="5">
+        <v>1933</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="3">
+        <v>4478</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1865</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="7">
+        <v>1854</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1854</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="3">
+        <v>8848</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1953</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="3">
+        <v>4167</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1931</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="3">
+        <v>3755</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1889</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="3">
+        <v>2655</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1796</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="3">
+        <v>2502</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1923</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="3">
+        <v>6961</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1934</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="3">
+        <v>7723</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="3">
+        <v>1985</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="3">
+        <v>3404</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1842</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="3">
+        <v>2063</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1906</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="B14" s="3">
+        <v>7439</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="3">
+        <v>1931</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="3">
+        <v>1895</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="D15" s="3">
+        <v>1929</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="3">
+        <v>3724</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="3">
+        <v>1894</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E18" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="2"/>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E18" xr:uid="{56986E0B-A4A6-4723-A20F-D2A7B21D0681}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E18">
-      <sortCondition ref="A1:A18"/>
+  <autoFilter ref="A1:E16" xr:uid="{56986E0B-A4A6-4723-A20F-D2A7B21D0681}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E16">
+      <sortCondition ref="A1:A16"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E9647E8-66DC-4ED7-9D1E-DC0058036050}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="40.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
new excel for geography
</commit_message>
<xml_diff>
--- a/SchVictorina.WebAPI/Config/mountains.xlsx
+++ b/SchVictorina.WebAPI/Config/mountains.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\schvictorina\schvictorina\SchVictorina.WebAPI\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{717FBB7B-EEAC-45C9-8722-52CFB2D3DE98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57767795-4269-479F-8C14-266704E40169}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{58996942-A194-4CF7-8E0B-222C89F5D031}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Вопросы" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Данные!$A$1:$E$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Данные!$A$1:$E$15</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="43">
   <si>
     <t>Название</t>
   </si>
@@ -90,9 +90,6 @@
   </si>
   <si>
     <t>Южные Альпы</t>
-  </si>
-  <si>
-    <t>Водораздельный хребет</t>
   </si>
   <si>
     <t>Альпы</t>
@@ -177,7 +174,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -197,14 +194,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF202122"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFBDC1C6"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -243,7 +232,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -251,7 +240,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
@@ -568,23 +556,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56986E0B-A4A6-4723-A20F-D2A7B21D0681}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="3"/>
+    <col min="1" max="1" width="24" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -592,7 +580,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -601,7 +589,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -609,7 +597,7 @@
         <v>4509</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" s="5">
         <v>1933</v>
@@ -618,15 +606,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="3">
         <v>4478</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" s="3">
         <v>1865</v>
@@ -635,234 +623,217 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="7">
-        <v>1854</v>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="3">
+        <v>8848</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="D4" s="3">
-        <v>1854</v>
+        <v>1953</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B5" s="3">
-        <v>8848</v>
+        <v>4167</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D5" s="3">
-        <v>1953</v>
+        <v>1931</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="B6" s="3">
-        <v>4167</v>
+        <v>3755</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D6" s="3">
-        <v>1931</v>
+        <v>1889</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>26</v>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="B7" s="3">
-        <v>3755</v>
+        <v>2655</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D7" s="3">
-        <v>1889</v>
+        <v>1796</v>
       </c>
       <c r="E7" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="3">
+        <v>2502</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1923</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="3">
+        <v>6961</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1934</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="3">
+        <v>7723</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1985</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="3">
-        <v>2655</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="3">
-        <v>1796</v>
-      </c>
-      <c r="E8" s="3" t="s">
+      <c r="B11" s="3">
+        <v>3404</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="3">
+        <v>1842</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="3">
-        <v>2502</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="3">
-        <v>1923</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="3">
-        <v>6961</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="3">
-        <v>1934</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="3">
-        <v>7723</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="3">
-        <v>1985</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B12" s="3">
-        <v>3404</v>
+        <v>2063</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="D12" s="3">
-        <v>1842</v>
+        <v>1906</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="3">
+        <v>7439</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1931</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="3">
+        <v>1895</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="3">
-        <v>2063</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="3">
-        <v>1906</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="3">
-        <v>7439</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="D14" s="3">
-        <v>1931</v>
+        <v>1929</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
-        <v>11</v>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="B15" s="3">
-        <v>1895</v>
+        <v>3724</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="D15" s="3">
-        <v>1929</v>
+        <v>1894</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="3">
-        <v>3724</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D16" s="3">
-        <v>1894</v>
-      </c>
-      <c r="E16" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="1"/>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E16" xr:uid="{56986E0B-A4A6-4723-A20F-D2A7B21D0681}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E16">
-      <sortCondition ref="A1:A16"/>
+  <autoFilter ref="A1:E15" xr:uid="{56986E0B-A4A6-4723-A20F-D2A7B21D0681}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E15">
+      <sortCondition ref="A1:A15"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -878,38 +849,38 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="9" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>36</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -921,9 +892,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -931,29 +902,29 @@
       <c r="D3" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="7" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="7" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" t="s">
         <v>41</v>
       </c>
-      <c r="C5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>1</v>
       </c>
       <c r="F5" t="s">

</xml_diff>